<commit_message>
download is now almost working - -when clicking on download the file gets to be saved
</commit_message>
<xml_diff>
--- a/timeentrydownload.xlsx
+++ b/timeentrydownload.xlsx
@@ -473,32 +473,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-05-22 00:00:00</t>
+          <t>2024-05-08 00:00:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4:07:00</t>
+          <t>4:40:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7:10:00</t>
+          <t>5:41:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-22 01:04:37</t>
+          <t>2024-05-22 01:37:38</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-05-22 01:04:37</t>
+          <t>2024-05-22 01:37:38</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -547,69 +547,69 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-05-27 00:00:00</t>
+          <t>2024-05-21 00:00:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4:29:00</t>
+          <t>15:57:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>7:32:00</t>
+          <t>18:00:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-05-22 01:26:23</t>
+          <t>2024-05-22 01:55:36</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-05-22 01:26:23</t>
+          <t>2024-05-22 01:55:36</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>johndoe</t>
+          <t>avisemah</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-05-28 00:00:00</t>
+          <t>2024-05-22 00:00:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3:36:00</t>
+          <t>4:07:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5:38:00</t>
+          <t>7:10:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-05-22 01:35:20</t>
+          <t>2024-05-22 01:04:37</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-05-22 01:35:20</t>
+          <t>2024-05-22 01:04:37</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -621,32 +621,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-05-08 00:00:00</t>
+          <t>2024-05-27 00:00:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4:40:00</t>
+          <t>4:29:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5:41:00</t>
+          <t>7:32:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024-05-22 01:37:38</t>
+          <t>2024-05-22 01:26:23</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-05-22 01:37:38</t>
+          <t>2024-05-22 01:26:23</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -658,37 +658,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-05-21 00:00:00</t>
+          <t>2024-05-28 00:00:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15:57:00</t>
+          <t>3:36:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>18:00:00</t>
+          <t>5:38:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024-05-22 01:55:36</t>
+          <t>2024-05-22 01:35:20</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-05-22 01:55:36</t>
+          <t>2024-05-22 01:35:20</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>avisemah</t>
+          <t>johndoe</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
able to donload a file with time entry results from a to z
</commit_message>
<xml_diff>
--- a/timeentrydownload.xlsx
+++ b/timeentrydownload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +473,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-05-08 00:00:00</t>
+          <t>2024-05-27 00:00:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4:40:00</t>
+          <t>4:29:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5:41:00</t>
+          <t>7:32:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-22 01:37:38</t>
+          <t>2024-05-22 01:26:23</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-05-22 01:37:38</t>
+          <t>2024-05-22 01:26:23</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -510,183 +510,35 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-05-14 00:00:00</t>
+          <t>2024-05-28 00:00:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5:09:00</t>
+          <t>3:36:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6:10:00</t>
+          <t>5:38:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-05-22 01:05:45</t>
+          <t>2024-05-22 01:35:20</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-05-22 01:05:45</t>
+          <t>2024-05-22 01:35:20</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>johndoe</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2024-05-21 00:00:00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>15:57:00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18:00:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:55:36</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:55:36</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>avisemah</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2024-05-22 00:00:00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4:07:00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>7:10:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:04:37</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:04:37</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>johndoe</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2024-05-27 00:00:00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>4:29:00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>7:32:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:26:23</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:26:23</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>johndoe</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2024-05-28 00:00:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>3:36:00</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5:38:00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:35:20</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:35:20</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>johndoe</t>
         </is>

</xml_diff>

<commit_message>
working on single time entry perfomed by admin --added drop donw of employees. it's working to the extent that admin can create an entry for an employee and do the overriding
</commit_message>
<xml_diff>
--- a/timeentrydownload.xlsx
+++ b/timeentrydownload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,78 +469,61 @@
           <t>uname</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>employeeid</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-05-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12:04:58</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-05-27 12:05:15</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024-05-27 12:05:15</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-05-27 00:00:00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>4:29:00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>7:32:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:26:23</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:26:23</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>johndoe</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-05-28 00:00:00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3:36:00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>5:38:00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:35:20</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-05-22 01:35:20</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>johndoe</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>alexa rodrig</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added favicon and password hashing
</commit_message>
<xml_diff>
--- a/timeentrydownload.xlsx
+++ b/timeentrydownload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>name</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>hours_worked</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,6 +531,11 @@
           <t>Avi Semah</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2:02:00</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -573,6 +583,11 @@
           <t>alexa rodrig</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2:53:24</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -620,6 +635,11 @@
           <t>erit gridnev</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0:00:48</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -667,6 +687,11 @@
           <t>Anthony zevek</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1:03:22</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -712,6 +737,427 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>alexa rodrig</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0:00:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18:32:53</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-05-31 18:33:02</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-05-31 18:33:02</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>alexa rodrig</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-1 day, 5:27:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>18:48:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>18:53:44</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-05-31 18:48:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-05-31 22:53:44</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>erit gridnev</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0:05:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>22:23:26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>23:53:33</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-05-31 22:23:26</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-06-01 03:53:33</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>1:30:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>23:21:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:21:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:21:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23:22:11</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>23:22:47</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:22:11</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:22:47</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0:00:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>23:46:30</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>23:50:27</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-06-01 03:46:30</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:50:27</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0:03:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>23:51:23</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>23:58:08</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:51:23</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-05-31 23:58:08</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0:06:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-06-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0:08:21</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0:09:10</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-06-01 04:08:22</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024-06-01 04:09:11</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0:00:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
before adding email button to where we have donwlaod
</commit_message>
<xml_diff>
--- a/timeentrydownload.xlsx
+++ b/timeentrydownload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>idtimeentry</t>
+          <t>start_date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>start_date</t>
+          <t>start_time</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>start_time</t>
+          <t>end_time</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>end_time</t>
+          <t>employeeid</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>created</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>last_updated</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>uname</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>employeeid</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>hours_worked</t>
         </is>
@@ -488,52 +468,128 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>2024-06-04 00:00:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>16:42:15</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>16:51:12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>erit gridnev</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0:08:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>2024-06-04 00:00:00</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>16:43:26</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>16:56:00</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-06-04 16:43:26</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-06-04 16:56:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Avi Semah</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>0:12:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-06-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16:59:46</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17:26:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OREN LAVI</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0:26:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-06-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>17:23:50</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>17:24:17</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Avi Semah</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0:00:27</t>
         </is>
       </c>
     </row>

</xml_diff>